<commit_message>
Dec 05 3:27 PM
</commit_message>
<xml_diff>
--- a/assets/public/products_partten.xlsx
+++ b/assets/public/products_partten.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t xml:space="preserve">quantity_in_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manufacturing_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expiry_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
   </si>
 </sst>
 </file>
@@ -107,13 +119,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -133,31 +153,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dec 05 10:50 PM
</commit_message>
<xml_diff>
--- a/assets/public/products_partten.xlsx
+++ b/assets/public/products_partten.xlsx
@@ -20,30 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity_in_stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity_in_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manufacturing_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expiry_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit</t>
   </si>
 </sst>
 </file>
@@ -119,13 +98,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -156,7 +139,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,27 +155,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>